<commit_message>
2511221848 - COMMON_TICKERS (Commented) and .env default values updated
</commit_message>
<xml_diff>
--- a/backend/docs/New Control Panel Layout.xlsx
+++ b/backend/docs/New Control Panel Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Other computers\My Computer\Documents\GitHub\Put-Oportunity-Finder\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A06C55-6B45-45F7-BADA-5B9278763804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193DACE2-D05D-44E5-8738-CB9CF80A7D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="170" yWindow="150" windowWidth="20980" windowHeight="19170" xr2:uid="{0C5663A8-B1CC-4D10-9A2E-A378A4701CA6}"/>
+    <workbookView xWindow="18840" yWindow="3000" windowWidth="14140" windowHeight="12890" activeTab="1" xr2:uid="{0C5663A8-B1CC-4D10-9A2E-A378A4701CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
   </sheetPr>
   <dimension ref="B1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1351,8 +1351,8 @@
   </sheetPr>
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="27">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="J21" s="27"/>
       <c r="M21" s="15"/>

</xml_diff>